<commit_message>
Cleaned and loaded the Housing Price Index UK and London file into my database.
</commit_message>
<xml_diff>
--- a/LondonDataProject/data/raw/housing-price-index-UK-London.xlsx
+++ b/LondonDataProject/data/raw/housing-price-index-UK-London.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mahamadoucamara/Documents/learning-data-engineering/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mahamadoucamara/Documents/Analysis-Of-London-Public-Transportation-System-And-Its-Impact-On-Economic-And-Social/LondonDataProject/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE95371-0738-9048-95CD-72CED8736BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA5E56F-1B2C-9549-BB78-F8A2F55417A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="20720" windowHeight="13280" tabRatio="596" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4945,8 +4945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E354"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A330" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="8" topLeftCell="A328" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I347" sqref="I347"/>
     </sheetView>
   </sheetViews>

</xml_diff>